<commit_message>
created front end design
</commit_message>
<xml_diff>
--- a/Client Submitted Details/Project related questioner details.xlsx
+++ b/Client Submitted Details/Project related questioner details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divyam Shah\Downloads\FW_ ___SPAM___ Fwd_ ___SPAM___ Re_ ___SPAM___ Re_ Final scope of work and no regret quote for case investigation mobile app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c8d651133008e5f/Desktop/Dynamic Labz/Clients/Clients/Ericson Healthcare/Ericson-Healthcare/Client Submitted Details/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899CFA26-BFF4-40E1-8A4D-5135CE6595B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D105EE5-97C4-49DD-839B-02DBA1CF8D54}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,6 +1714,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1914,9 +1915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EEE8334-046D-4ED3-BA15-EDCEBDBE83DA}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2310,7 +2309,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2525,6 +2524,7 @@
     <mergeCell ref="A10:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2533,7 +2533,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>